<commit_message>
Aulas do primeiro módulo - operações aritméticas (resolução do exercício)
</commit_message>
<xml_diff>
--- a/exercicio-proposto-operacoes-aritmeticas.xlsx
+++ b/exercicio-proposto-operacoes-aritmeticas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>MÊS</t>
   </si>
@@ -104,20 +104,51 @@
   </si>
   <si>
     <t>VARIAÇÃO EM RELAÇÃO À META</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Formulas utilizadas nos cálculos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Gasto com combustível por veículo: Litros * Preço combustível (trancamento da célula).
+ Gasto total = Gasto com combustível + Gasto com peças + Gasto com serviços
+ Gasto por Km = Gasto Total / Km Rodados
+ Rendimento de combustível = Km Rodados / Litros
+ Variação da meta de Gasto/Km = (Gasto por Km / Meta de Gasto/Km) - 1 (trancamento da célula).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.000"/>
     <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="_-&quot;R$&quot;* #,##0.0000_-;\-&quot;R$&quot;* #,##0.0000_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +207,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13.95"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -317,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -420,6 +467,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,7 +792,7 @@
   <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,16 +883,28 @@
       <c r="D5" s="5">
         <v>142.19999999999999</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="20">
+        <f>D5*$H$3</f>
+        <v>696.63779999999997</v>
+      </c>
       <c r="F5" s="20">
         <v>500</v>
       </c>
       <c r="G5" s="20">
         <v>350</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="5"/>
+      <c r="H5" s="20">
+        <f>E5+F5+G5</f>
+        <v>1546.6378</v>
+      </c>
+      <c r="I5" s="20">
+        <f>H5/C5</f>
+        <v>1.1456576296296297</v>
+      </c>
+      <c r="J5" s="5">
+        <f>C5/D5</f>
+        <v>9.4936708860759502</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -850,16 +916,28 @@
       <c r="D6" s="5">
         <v>224.2</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="20">
+        <f t="shared" ref="E6:E8" si="0">D6*$H$3</f>
+        <v>1098.3558</v>
+      </c>
       <c r="F6" s="20">
         <v>250</v>
       </c>
       <c r="G6" s="20">
         <v>35</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="5"/>
+      <c r="H6" s="20">
+        <f>E6+F6+G6</f>
+        <v>1383.3558</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" ref="I6:I8" si="1">H6/C6</f>
+        <v>0.7094132307692308</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" ref="J6:J9" si="2">C6/D6</f>
+        <v>8.6975914362176638</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -871,16 +949,28 @@
       <c r="D7" s="5">
         <v>247</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="20">
+        <f t="shared" si="0"/>
+        <v>1210.0530000000001</v>
+      </c>
       <c r="F7" s="20">
         <v>180</v>
       </c>
       <c r="G7" s="20">
         <v>56</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="5"/>
+      <c r="H7" s="20">
+        <f>E7+F7+G7</f>
+        <v>1446.0530000000001</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" si="1"/>
+        <v>0.57383055555555562</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="2"/>
+        <v>10.20242914979757</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -892,29 +982,68 @@
       <c r="D8" s="5">
         <v>117.5</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>575.63250000000005</v>
+      </c>
       <c r="F8" s="20">
         <v>95</v>
       </c>
       <c r="G8" s="20">
         <v>0</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="5"/>
+      <c r="H8" s="20">
+        <f>E8+F8+G8</f>
+        <v>670.63250000000005</v>
+      </c>
+      <c r="I8" s="20">
+        <f t="shared" si="1"/>
+        <v>0.47562588652482274</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="7"/>
+      <c r="C9" s="8">
+        <f>SUM(C5:C8)</f>
+        <v>7230</v>
+      </c>
+      <c r="D9" s="7">
+        <f>D5+D6+D7+D8</f>
+        <v>730.9</v>
+      </c>
+      <c r="E9" s="36">
+        <f>E5+E6+E7+E8</f>
+        <v>3580.6791000000003</v>
+      </c>
+      <c r="F9" s="19">
+        <f>F5+F6+F7+F8</f>
+        <v>1025</v>
+      </c>
+      <c r="G9" s="19">
+        <f>G5+G6+G7</f>
+        <v>441</v>
+      </c>
+      <c r="H9" s="19">
+        <f>H5+H6+H7+H8</f>
+        <v>5046.6790999999994</v>
+      </c>
+      <c r="I9" s="19">
+        <f>H9/C9</f>
+        <v>0.69801923928077447</v>
+      </c>
+      <c r="J9" s="7">
+        <f>C9/D9</f>
+        <v>9.8919140785333148</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G10" s="35"/>
     </row>
     <row r="12" spans="2:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="28" t="s">
@@ -922,6 +1051,13 @@
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
+      <c r="F12" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
@@ -932,7 +1068,11 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
     </row>
     <row r="14" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
@@ -945,7 +1085,11 @@
         <v>25</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="G14" s="13"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
@@ -954,9 +1098,16 @@
       <c r="C15" s="21">
         <v>0.59599999999999997</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12">
+        <f>C15/$D$13-1</f>
+        <v>2.7586206896551779E-2</v>
+      </c>
       <c r="E15" s="9"/>
-      <c r="G15" s="13"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
@@ -965,47 +1116,69 @@
       <c r="C16" s="21">
         <v>0.58199999999999996</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="12">
+        <f t="shared" ref="D16:D19" si="3">C16/$D$13-1</f>
+        <v>3.4482758620688614E-3</v>
+      </c>
       <c r="E16" s="9"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="21">
         <v>0.57199999999999995</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="12">
+        <f t="shared" si="3"/>
+        <v>-1.379310344827589E-2</v>
+      </c>
       <c r="E17" s="9"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="21">
         <v>0.61199999999999999</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12">
+        <f t="shared" si="3"/>
+        <v>5.5172413793103559E-2</v>
+      </c>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="21">
         <v>0.64549999999999996</v>
       </c>
-      <c r="D19" s="12"/>
+      <c r="D19" s="12">
+        <f t="shared" si="3"/>
+        <v>0.11293103448275854</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F12:J17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1013,7 +1186,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>